<commit_message>
game project day 03
</commit_message>
<xml_diff>
--- a/detail.xlsx
+++ b/detail.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="131">
   <si>
     <t>Main</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1639,33 +1639,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>배경(Stage) 만들기</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t/>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>기본 캐릭터 움직임 코드 작성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격 코드 작성 시작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>몬스터 움직임  코드 작성 시작</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>아이템 관련 코드 작성 및 마무리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2504,50 +2477,81 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Character</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">const unsigned short * Man[] = {man_01,}; </t>
+  </si>
+  <si>
+    <t>Expect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터 불러오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배경 영역 나눠 작성하기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ongoing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뛰기, 걷기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가만히 있기, 다가오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배경움직임 자연스럽게 만들기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배경 로드문제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 움직임  코드 작성 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 캐릭터 움직임 코드 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>배경(Stage) 만들기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>캐릭터 만들기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Character</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">const unsigned short * Man[] = {man_01,}; </t>
-  </si>
-  <si>
-    <t>Expect</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>캐릭터 불러오기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배경 영역 나눠 작성하기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ongoing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>뛰기, 걷기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>가만히 있기, 다가오기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배경움직임 자연스럽게 만들기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>배경 로드문제</t>
+    <t>공격 코드 작성 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몬스터 움직임  코드 작성 시작</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2984,12 +2988,24 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3001,18 +3017,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3572,28 +3576,28 @@
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
     </row>
     <row r="3" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
@@ -3632,18 +3636,18 @@
       <c r="B5" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
       <c r="O5" s="17"/>
     </row>
     <row r="6" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3672,36 +3676,36 @@
       <c r="C7" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
       <c r="O7" s="17"/>
     </row>
     <row r="8" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
       <c r="O8" s="17"/>
     </row>
     <row r="9" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3714,19 +3718,19 @@
       <c r="C9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
     </row>
     <row r="10" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
@@ -3735,18 +3739,18 @@
       <c r="C10" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
       <c r="O10" s="17"/>
     </row>
     <row r="11" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3760,33 +3764,33 @@
         <v>59</v>
       </c>
       <c r="D11" s="21"/>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
       <c r="O11" s="17"/>
     </row>
     <row r="12" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
-      <c r="N12" s="46"/>
+      <c r="E12" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E13" s="14"/>
@@ -3801,12 +3805,12 @@
       <c r="N13" s="14"/>
     </row>
     <row r="14" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="46"/>
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -3833,7 +3837,7 @@
     </row>
     <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
@@ -4085,6 +4089,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="E1:M2"/>
+    <mergeCell ref="E5:N5"/>
     <mergeCell ref="E14:H14"/>
     <mergeCell ref="E8:N8"/>
     <mergeCell ref="E10:N10"/>
@@ -4092,8 +4098,6 @@
     <mergeCell ref="E9:O9"/>
     <mergeCell ref="E11:N11"/>
     <mergeCell ref="E12:N12"/>
-    <mergeCell ref="E1:M2"/>
-    <mergeCell ref="E5:N5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4107,7 +4111,7 @@
   <dimension ref="B2:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4125,13 +4129,13 @@
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
@@ -4150,27 +4154,27 @@
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="15"/>
       <c r="C5" s="14"/>
-      <c r="D5" s="23" t="s">
-        <v>87</v>
+      <c r="D5" s="39" t="s">
+        <v>127</v>
       </c>
       <c r="E5" s="39" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="15"/>
       <c r="C6" s="14"/>
-      <c r="D6" s="23" t="s">
-        <v>118</v>
+      <c r="D6" s="40" t="s">
+        <v>128</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F6" s="42" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -4178,15 +4182,15 @@
       <c r="C7" s="14"/>
       <c r="D7" s="23"/>
       <c r="E7" s="40" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F7" s="42"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="15"/>
       <c r="C8" s="14"/>
-      <c r="D8" s="23" t="s">
-        <v>88</v>
+      <c r="D8" s="40" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
@@ -4199,42 +4203,42 @@
         <v>43676</v>
       </c>
       <c r="C10" s="14"/>
-      <c r="D10" s="23" t="s">
-        <v>89</v>
+      <c r="D10" s="40" t="s">
+        <v>129</v>
       </c>
       <c r="E10" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="39" t="s">
         <v>124</v>
-      </c>
-      <c r="F10" s="39" t="s">
-        <v>128</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="15"/>
-      <c r="D11" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>90</v>
+      <c r="D11" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="F11" s="39" t="s">
+        <v>125</v>
       </c>
       <c r="G11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="15"/>
       <c r="C12" s="14"/>
       <c r="D12" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>126</v>
       </c>
       <c r="G12" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
@@ -4248,28 +4252,28 @@
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="15"/>
       <c r="C15" s="21"/>
       <c r="D15" s="23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="15"/>
       <c r="C16" s="14"/>
       <c r="D16" s="23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="15"/>
       <c r="C17" s="14"/>
       <c r="D17" s="23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
@@ -4283,19 +4287,19 @@
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="23" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="15"/>
       <c r="D20" s="23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="15"/>
       <c r="D21" s="23" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -4307,13 +4311,13 @@
         <v>43679</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" s="15"/>
       <c r="D24" s="23" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -4325,16 +4329,16 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" s="24" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="36" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D28" s="37" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
@@ -4375,7 +4379,7 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
@@ -4389,7 +4393,7 @@
     </row>
     <row r="6" spans="2:2" ht="33" x14ac:dyDescent="0.3">
       <c r="B6" s="29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.3">
@@ -4397,7 +4401,7 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" s="29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.3">
@@ -4405,7 +4409,7 @@
     </row>
     <row r="10" spans="2:2" ht="33" x14ac:dyDescent="0.3">
       <c r="B10" s="30" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
@@ -4413,7 +4417,7 @@
     </row>
     <row r="12" spans="2:2" ht="33" x14ac:dyDescent="0.3">
       <c r="B12" s="31" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.3">
@@ -4421,7 +4425,7 @@
     </row>
     <row r="14" spans="2:2" ht="33" x14ac:dyDescent="0.3">
       <c r="B14" s="29" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.3">
@@ -4429,7 +4433,7 @@
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" s="29" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
@@ -4437,7 +4441,7 @@
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="32" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
@@ -4445,7 +4449,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="33" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -4469,12 +4473,12 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
game project day 04
</commit_message>
<xml_diff>
--- a/detail.xlsx
+++ b/detail.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="135">
   <si>
     <t>Main</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2552,6 +2552,22 @@
   </si>
   <si>
     <t>몬스터 움직임  코드 작성 시작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Move / Draw 함수 분리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>좀비 움직임 코드 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영역 계산 오류 수정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>* 맵, 플레이어, 좀비</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2988,6 +3004,15 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3008,15 +3033,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3576,28 +3592,28 @@
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
@@ -3636,18 +3652,18 @@
       <c r="B5" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
-      <c r="M5" s="53"/>
-      <c r="N5" s="53"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
       <c r="O5" s="17"/>
     </row>
     <row r="6" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3676,36 +3692,36 @@
       <c r="C7" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
       <c r="O7" s="17"/>
     </row>
     <row r="8" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="47" t="s">
+      <c r="E8" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
       <c r="O8" s="17"/>
     </row>
     <row r="9" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3718,19 +3734,19 @@
       <c r="C9" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="49"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
     </row>
     <row r="10" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14" t="s">
@@ -3739,18 +3755,18 @@
       <c r="C10" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
       <c r="O10" s="17"/>
     </row>
     <row r="11" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -3764,33 +3780,33 @@
         <v>59</v>
       </c>
       <c r="D11" s="21"/>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
       <c r="O11" s="17"/>
     </row>
     <row r="12" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="50" t="s">
+      <c r="E12" s="53" t="s">
         <v>109</v>
       </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="50"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="53"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E13" s="14"/>
@@ -3805,12 +3821,12 @@
       <c r="N13" s="14"/>
     </row>
     <row r="14" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="46"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
       <c r="J14" s="3"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -4110,8 +4126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4268,20 +4284,32 @@
       <c r="D16" s="23" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="39" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="15"/>
       <c r="C17" s="14"/>
       <c r="D17" s="23" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="15"/>
       <c r="C18" s="14"/>
       <c r="D18" s="23"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="15">
         <v>43678</v>
       </c>
@@ -4290,23 +4318,23 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="15"/>
       <c r="D20" s="23" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="15"/>
       <c r="D21" s="23" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="15"/>
       <c r="D22" s="23"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="15">
         <v>43679</v>
       </c>
@@ -4314,20 +4342,20 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="15"/>
       <c r="D24" s="23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="15"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="15"/>
       <c r="D26" s="14"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="24" t="s">
         <v>96</v>
       </c>
@@ -4336,22 +4364,22 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D28" s="37" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D29" s="34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D30" s="38" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="D31" s="35" t="s">
         <v>79</v>
       </c>

</xml_diff>